<commit_message>
Added comparable interface to Planet, NPCs and Items, meaning whenever their list is printed, it will be sorted by reference number. Also formatted (using the IDE command) all the documents. Next up: looking at the placement NPC bug, perhaps it is not even necessary? And also, when should NPCs move?
</commit_message>
<xml_diff>
--- a/Zuul framework/data/alpha_centauri/readme.xlsx
+++ b/Zuul framework/data/alpha_centauri/readme.xlsx
@@ -452,8 +452,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="T4" sqref="T4"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -535,7 +535,7 @@
         <v>29</v>
       </c>
       <c r="N3">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="P3">
         <v>2</v>
@@ -638,6 +638,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>